<commit_message>
Avance 07 de noviembre de 2019
</commit_message>
<xml_diff>
--- a/MatrizODMedellin Modelos/MatrizOD12Ptos.xlsx
+++ b/MatrizODMedellin Modelos/MatrizOD12Ptos.xlsx
@@ -5,23 +5,24 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williz/Dropbox/Doctorado/Tesis Doctorado/Avances Tesis/Analisis Datos Tesis/MatrizODMedellin Modelos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williz/Desktop/ModelosED/MatrizODMedellin Modelos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96E6F5C5-1887-BA42-A5FA-F03DC3205142}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAE9775-18D5-CA4E-9A13-C8264E3ED86F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24000" windowHeight="8780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24000" windowHeight="12020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ODFull" sheetId="1" r:id="rId1"/>
     <sheet name="ODMatriz" sheetId="2" r:id="rId2"/>
+    <sheet name="Puentes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
   <si>
     <t>Latitud</t>
   </si>
@@ -150,6 +151,42 @@
   </si>
   <si>
     <t>Universidad de Antioquia - Zona Oriental</t>
+  </si>
+  <si>
+    <t>Madre Laura</t>
+  </si>
+  <si>
+    <t>Mico</t>
+  </si>
+  <si>
+    <t>Barranquilla</t>
+  </si>
+  <si>
+    <t>Minorista</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>San Juan</t>
+  </si>
+  <si>
+    <t>La 33</t>
+  </si>
+  <si>
+    <t>Av Guayabal</t>
+  </si>
+  <si>
+    <t>La 30</t>
+  </si>
+  <si>
+    <t>La 10</t>
+  </si>
+  <si>
+    <t>Gilberto Echeverri</t>
+  </si>
+  <si>
+    <t>Aguacatala</t>
   </si>
 </sst>
 </file>
@@ -470,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection sqref="A1:C41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -939,10 +976,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -985,24 +1022,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1">
-        <v>6.2555750000000003</v>
+        <v>6.2790699999999999</v>
       </c>
       <c r="C4" s="1">
-        <v>-75.601588000000007</v>
+        <v>-75.571295000000006</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>6.2444800000000003</v>
+        <v>6.2413080000000001</v>
       </c>
       <c r="C5" s="1">
-        <v>-75.589434999999995</v>
+        <v>-75.587549999999993</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1018,126 +1055,135 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>6.2188299999999996</v>
+        <v>6.2569600000000003</v>
       </c>
       <c r="C7" s="1">
-        <v>-75.586550000000003</v>
+        <v>-75.591989999999996</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1">
-        <v>6.2090420000000002</v>
+        <v>6.2078949999999997</v>
       </c>
       <c r="C8" s="1">
-        <v>-75.567779999999999</v>
+        <v>-75.590900000000005</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1">
-        <v>6.2292639999999997</v>
+        <v>6.2188299999999996</v>
       </c>
       <c r="C9" s="1">
-        <v>-75.570485000000005</v>
+        <v>-75.586550000000003</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1">
-        <v>6.2448639999999997</v>
+        <v>6.2822560000000003</v>
       </c>
       <c r="C10" s="1">
-        <v>-75.577209999999994</v>
+        <v>-75.561384000000004</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1">
-        <v>6.2536389999999997</v>
+        <v>6.2665240000000004</v>
       </c>
       <c r="C11" s="1">
-        <v>-75.564184999999995</v>
+        <v>-75.563665999999998</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1">
-        <v>6.2665240000000004</v>
+        <v>6.2616630000000004</v>
       </c>
       <c r="C12" s="1">
-        <v>-75.563665999999998</v>
+        <v>-75.565776999999997</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1">
-        <v>6.2822560000000003</v>
+        <v>6.2536389999999997</v>
       </c>
       <c r="C13" s="1">
-        <v>-75.561384000000004</v>
+        <v>-75.564184999999995</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1">
+        <v>6.2523210000000002</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-75.567431999999997</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1">
+        <v>6.2357120000000004</v>
+      </c>
+      <c r="C15" s="1">
+        <v>-75.569559999999996</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="1">
+        <v>6.2090420000000002</v>
+      </c>
+      <c r="C16" s="1">
+        <v>-75.567779999999999</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6.223611</v>
+      </c>
+      <c r="C17" s="1">
+        <v>-75.574438000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-    </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
@@ -1173,11 +1219,6 @@
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-    </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
@@ -1188,40 +1229,45 @@
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+    </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
@@ -1233,10 +1279,201 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79D0D78-7E58-A940-A7F6-6718BF68E7E3}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2">
+        <v>6.2861830000000003</v>
+      </c>
+      <c r="C2">
+        <v>-75.565989000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3">
+        <v>6.2758929999999999</v>
+      </c>
+      <c r="C3">
+        <v>-75.569779999999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4">
+        <v>6.2652020000000004</v>
+      </c>
+      <c r="C4">
+        <v>-75.572181999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5">
+        <v>6.2608949999999997</v>
+      </c>
+      <c r="C5">
+        <v>-75.573702999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>6.2542119999999999</v>
+      </c>
+      <c r="C6">
+        <v>-75.577287999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7">
+        <v>6.24796</v>
+      </c>
+      <c r="C7">
+        <v>-75.580280999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8">
+        <v>6.2396450000000003</v>
+      </c>
+      <c r="C8">
+        <v>-75.577397000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>6.2368969999999999</v>
+      </c>
+      <c r="C9">
+        <v>-75.576466999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10">
+        <v>6.2313780000000003</v>
+      </c>
+      <c r="C10">
+        <v>-75.575670000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11">
+        <v>6.2135939999999996</v>
+      </c>
+      <c r="C11">
+        <v>-75.578073000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12">
+        <v>6.2040309999999996</v>
+      </c>
+      <c r="C12">
+        <v>-75.579593000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13">
+        <v>6.1952930000000004</v>
+      </c>
+      <c r="C13">
+        <v>-75.581541999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>